<commit_message>
ARKCORR-22 Minor changes to the dueDate setting for the 'Release' queue.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\Documents\correspondence-management\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -203,10 +203,10 @@
     <t>Set Due Date Release Queue</t>
   </si>
   <si>
-    <t>setDueDate, toDate(java.time.LocalDate.now())</t>
-  </si>
-  <si>
-    <t>dueDate == null &amp;&amp; queue.name == "Release"</t>
+    <t>queue.name == "Release"</t>
+  </si>
+  <si>
+    <t>setDueDate, null</t>
   </si>
 </sst>
 </file>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1197,10 +1197,10 @@
         <v>54</v>
       </c>
       <c r="C31" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ARKCORR-22 Added elvis operator to drools rules.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -188,25 +188,25 @@
     <t>setDueDate, toDate(java.time.LocalDate.now().plusDays(2))</t>
   </si>
   <si>
-    <t>queue.name == "Intake"</t>
-  </si>
-  <si>
-    <t>queue.name == "Fulfill"</t>
-  </si>
-  <si>
-    <t>queue.name == "Supervisor Approval"</t>
-  </si>
-  <si>
-    <t>queue.name == "Executive Approval"</t>
-  </si>
-  <si>
     <t>Set Due Date Release Queue</t>
   </si>
   <si>
-    <t>queue.name == "Release"</t>
-  </si>
-  <si>
     <t>setDueDate, null</t>
+  </si>
+  <si>
+    <t>queue?.name == "Intake"</t>
+  </si>
+  <si>
+    <t>queue?.name == "Fulfill"</t>
+  </si>
+  <si>
+    <t>queue?.name == "Supervisor Approval"</t>
+  </si>
+  <si>
+    <t>queue?.name == "Executive Approval"</t>
+  </si>
+  <si>
+    <t>queue?.name == "Release"</t>
   </si>
 </sst>
 </file>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1149,7 +1149,7 @@
         <v>39</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>47</v>
@@ -1161,7 +1161,7 @@
         <v>40</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>48</v>
@@ -1173,7 +1173,7 @@
         <v>41</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>49</v>
@@ -1185,7 +1185,7 @@
         <v>42</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>49</v>
@@ -1194,13 +1194,13 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ARKCORR-25: Update rules to set queue enter date
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>RuleSet</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>queue?.name == "Release"</t>
+  </si>
+  <si>
+    <t>setQueueEnterDate, toDate(java.time.LocalDate.now())</t>
   </si>
 </sst>
 </file>
@@ -877,23 +880,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D31"/>
+  <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="C15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.3984375"/>
-    <col min="2" max="2" width="24.265625"/>
-    <col min="3" max="3" width="50.1328125"/>
-    <col min="4" max="4" width="100.3984375"/>
-    <col min="5" max="5" width="27.73046875"/>
-    <col min="6" max="1025" width="8.73046875"/>
+    <col min="1" max="1" width="19.42578125"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="50.140625"/>
+    <col min="4" max="4" width="100.42578125"/>
+    <col min="5" max="5" width="102.140625" customWidth="1"/>
+    <col min="6" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -903,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -913,7 +916,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -923,7 +926,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -933,7 +936,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -943,7 +946,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -953,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -963,7 +966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -973,7 +976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -983,7 +986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -993,7 +996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1003,7 +1006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1013,7 +1016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="285" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="300" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1023,7 +1026,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
@@ -1033,15 +1036,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="4" t="s">
@@ -1050,16 +1055,20 @@
       <c r="D18" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E18" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
@@ -1068,8 +1077,11 @@
       <c r="D20" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="E20" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -1082,8 +1094,11 @@
       <c r="D21" s="16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E21" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>22</v>
@@ -1094,8 +1109,9 @@
       <c r="D22" s="17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>25</v>
@@ -1106,8 +1122,9 @@
       <c r="D23" s="17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>28</v>
@@ -1118,8 +1135,9 @@
       <c r="D24" s="17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>31</v>
@@ -1130,8 +1148,9 @@
       <c r="D25" s="17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>34</v>
@@ -1142,8 +1161,9 @@
       <c r="D26" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>39</v>
@@ -1154,8 +1174,11 @@
       <c r="D27" s="17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E27" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>40</v>
@@ -1166,8 +1189,11 @@
       <c r="D28" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E28" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>41</v>
@@ -1178,8 +1204,11 @@
       <c r="D29" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E29" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
         <v>42</v>
@@ -1190,8 +1219,11 @@
       <c r="D30" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E30" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
         <v>50</v>
@@ -1201,6 +1233,9 @@
       </c>
       <c r="D31" s="17" t="s">
         <v>51</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1215,9 +1250,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1231,9 +1266,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Fixing rules with LocalDate problem
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
     <t>queue?.name == "Release"</t>
   </si>
   <si>
-    <t>setQueueEnterDate, toDate(java.time.LocalDate.now())</t>
+    <t>setQueueEnterDate, java.time.LocalDate.now()</t>
   </si>
 </sst>
 </file>
@@ -882,21 +882,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125"/>
-    <col min="2" max="2" width="24.28515625"/>
-    <col min="3" max="3" width="50.140625"/>
-    <col min="4" max="4" width="100.42578125"/>
-    <col min="5" max="5" width="102.140625" customWidth="1"/>
-    <col min="6" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="19.453125"/>
+    <col min="2" max="2" width="24.26953125"/>
+    <col min="3" max="3" width="50.1796875"/>
+    <col min="4" max="4" width="100.453125"/>
+    <col min="5" max="5" width="102.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -906,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -916,7 +915,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -926,7 +925,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -936,7 +935,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -946,7 +945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -956,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -966,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -976,7 +975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -986,7 +985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -996,7 +995,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1006,7 +1005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1016,7 +1015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="290" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1026,7 +1025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
@@ -1036,8 +1035,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
@@ -1046,7 +1045,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="4" t="s">
@@ -1059,7 +1058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
@@ -1068,7 +1067,7 @@
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
@@ -1081,7 +1080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>18</v>
       </c>
@@ -1098,7 +1097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>22</v>
@@ -1111,7 +1110,7 @@
       </c>
       <c r="E22" s="17"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>25</v>
@@ -1124,7 +1123,7 @@
       </c>
       <c r="E23" s="17"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>28</v>
@@ -1137,7 +1136,7 @@
       </c>
       <c r="E24" s="17"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>31</v>
@@ -1150,7 +1149,7 @@
       </c>
       <c r="E25" s="17"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>34</v>
@@ -1163,7 +1162,7 @@
       </c>
       <c r="E26" s="17"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>39</v>
@@ -1178,7 +1177,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>40</v>
@@ -1193,7 +1192,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>41</v>
@@ -1208,7 +1207,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
         <v>42</v>
@@ -1223,7 +1222,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
         <v>50</v>
@@ -1250,10 +1249,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.7109375"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1266,10 +1262,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.7109375"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
ARKCORR-18: Updating assigned Group when object moves to queues
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>RuleSet</t>
   </si>
@@ -159,6 +159,60 @@
   </si>
   <si>
     <t>java.time.ZoneId</t>
+  </si>
+  <si>
+    <t>setDueDate, toDate(java.time.LocalDate.now().plusDays(1))</t>
+  </si>
+  <si>
+    <t>setDueDate, toDate(java.time.LocalDate.now().plusDays(5))</t>
+  </si>
+  <si>
+    <t>setDueDate, toDate(java.time.LocalDate.now().plusDays(2))</t>
+  </si>
+  <si>
+    <t>Set Due Date Release Queue</t>
+  </si>
+  <si>
+    <t>setDueDate, null</t>
+  </si>
+  <si>
+    <t>queue?.name == "Intake"</t>
+  </si>
+  <si>
+    <t>queue?.name == "Fulfill"</t>
+  </si>
+  <si>
+    <t>queue?.name == "Supervisor Approval"</t>
+  </si>
+  <si>
+    <t>queue?.name == "Executive Approval"</t>
+  </si>
+  <si>
+    <t>queue?.name == "Release"</t>
+  </si>
+  <si>
+    <t>setQueueEnterDate, java.time.LocalDate.now()</t>
+  </si>
+  <si>
+    <t>Set Owning Group</t>
+  </si>
+  <si>
+    <t>owning group, ExecSec Intake</t>
+  </si>
+  <si>
+    <t>owning group, ExecSec Approval</t>
+  </si>
+  <si>
+    <t>owning group, ExecSec Release</t>
+  </si>
+  <si>
+    <t>addOrUpdateParticipant($caseFile, "$1", "$2");</t>
+  </si>
+  <si>
+    <t>com.armedia.acm.services.participants.model.AcmAssignedObject</t>
+  </si>
+  <si>
+    <t>com.armedia.acm.services.participants.model.AcmParticipant</t>
   </si>
   <si>
     <t>function String dateFormat(String fmt)
@@ -176,40 +230,36 @@
     EvaluationContext ec = new StandardEvaluationContext();
     Boolean evaluated = exp.getValue(ec, obj, Boolean.class);
     return evaluated;
+}
+function void addOrUpdateParticipant(AcmAssignedObject obj, String type, String id) 
+{
+    if  (obj.getParticipants() != null &amp;&amp; type != null)
+    {
+        boolean updated = false;
+        for (AcmParticipant p :  obj.getParticipants())
+        {
+             if (type.equals(p.getParticipantType()))
+             {
+                  p.setParticipantLdapId(id);
+                  updated = true;
+                  break;
+             }
+        }
+        if (!updated)
+        {
+            AcmParticipant p = new AcmParticipant();
+            p.setParticipantType(type);
+            p.setParticipantLdapId(id);
+            obj.getParticipants().add(p);
+        }
+    }
 }</t>
   </si>
   <si>
-    <t>setDueDate, toDate(java.time.LocalDate.now().plusDays(1))</t>
-  </si>
-  <si>
-    <t>setDueDate, toDate(java.time.LocalDate.now().plusDays(5))</t>
-  </si>
-  <si>
-    <t>setDueDate, toDate(java.time.LocalDate.now().plusDays(2))</t>
-  </si>
-  <si>
-    <t>Set Due Date Release Queue</t>
-  </si>
-  <si>
-    <t>setDueDate, null</t>
-  </si>
-  <si>
-    <t>queue?.name == "Intake"</t>
-  </si>
-  <si>
-    <t>queue?.name == "Fulfill"</t>
-  </si>
-  <si>
-    <t>queue?.name == "Supervisor Approval"</t>
-  </si>
-  <si>
-    <t>queue?.name == "Executive Approval"</t>
-  </si>
-  <si>
-    <t>queue?.name == "Release"</t>
-  </si>
-  <si>
-    <t>setQueueEnterDate, java.time.LocalDate.now()</t>
+    <t>owning group, Analyst - AG</t>
+  </si>
+  <si>
+    <t>owning group, Supervisor - AG</t>
   </si>
 </sst>
 </file>
@@ -880,22 +930,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E31"/>
+  <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125"/>
-    <col min="2" max="2" width="24.26953125"/>
-    <col min="3" max="3" width="50.1796875"/>
-    <col min="4" max="4" width="100.453125"/>
-    <col min="5" max="5" width="102.1796875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="50.140625"/>
+    <col min="4" max="4" width="100.42578125"/>
+    <col min="5" max="5" width="102.140625" customWidth="1"/>
+    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -905,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -915,7 +966,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -925,7 +976,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -935,7 +986,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -945,7 +996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -955,7 +1006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -965,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -975,7 +1026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -985,7 +1036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -995,7 +1046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1005,7 +1056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1015,226 +1066,277 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="290" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E22" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
+      <c r="F22" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B23" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E23" s="16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E24" s="17"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="17"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E25" s="17"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E26" s="17"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="E33" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>57</v>
+      <c r="F33" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1249,7 +1351,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1262,7 +1364,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
ARKCORR-32: Set Response Due Date
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>RuleSet</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Set Due Date Release Queue</t>
-  </si>
-  <si>
-    <t>setDueDate, null</t>
   </si>
   <si>
     <t>queue?.name == "Intake"</t>
@@ -260,6 +257,15 @@
   </si>
   <si>
     <t>owning group, Supervisor - AG</t>
+  </si>
+  <si>
+    <t>Set Response Due Date</t>
+  </si>
+  <si>
+    <t>responseDueDate == null</t>
+  </si>
+  <si>
+    <t>setResponseDueDate, java.time.LocalDate.now().plusDays(10)</t>
   </si>
 </sst>
 </file>
@@ -930,23 +936,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F33"/>
+  <dimension ref="A2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125"/>
-    <col min="2" max="2" width="24.28515625"/>
-    <col min="3" max="3" width="50.140625"/>
-    <col min="4" max="4" width="100.42578125"/>
-    <col min="5" max="5" width="102.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.453125"/>
+    <col min="2" max="2" width="24.26953125"/>
+    <col min="3" max="3" width="50.1796875"/>
+    <col min="4" max="4" width="100.453125"/>
+    <col min="5" max="5" width="102.1796875" customWidth="1"/>
     <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -956,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -966,7 +972,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -976,7 +982,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -986,7 +992,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -996,7 +1002,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1006,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1016,7 +1022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1026,7 +1032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1036,7 +1042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1046,7 +1052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1056,7 +1062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1066,37 +1072,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8" t="s">
@@ -1106,8 +1112,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -1117,7 +1123,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
@@ -1133,7 +1139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
@@ -1143,7 +1149,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="11" t="s">
@@ -1156,10 +1162,10 @@
         <v>17</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
@@ -1176,167 +1182,179 @@
         <v>21</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>48</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="1"/>
+      <c r="B34" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C34" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>60</v>
+      <c r="F34" s="17" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1351,7 +1369,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1364,7 +1382,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
AFDP-3021: Configuring assignee per queue
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>RuleSet</t>
   </si>
@@ -266,6 +266,21 @@
   </si>
   <si>
     <t>setResponseDueDate, java.time.LocalDate.now().plusDays(10)</t>
+  </si>
+  <si>
+    <t>assignee, sally-acm</t>
+  </si>
+  <si>
+    <t>assignee, ian-acm</t>
+  </si>
+  <si>
+    <t>assignee, samuel-acm</t>
+  </si>
+  <si>
+    <t>assignee, ann-acm</t>
+  </si>
+  <si>
+    <t>Set Assignee</t>
   </si>
 </sst>
 </file>
@@ -936,23 +951,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F34"/>
+  <dimension ref="A2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125"/>
-    <col min="2" max="2" width="24.26953125"/>
-    <col min="3" max="3" width="50.1796875"/>
-    <col min="4" max="4" width="100.453125"/>
-    <col min="5" max="5" width="102.1796875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="50.140625"/>
+    <col min="4" max="4" width="100.42578125"/>
+    <col min="5" max="5" width="102.140625" customWidth="1"/>
     <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -962,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -972,7 +988,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -982,7 +998,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -992,7 +1008,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1002,7 +1018,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1012,7 +1028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1022,7 +1038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1032,7 +1048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1042,7 +1058,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1052,7 +1068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1062,7 +1078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1072,7 +1088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1082,7 +1098,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1092,7 +1108,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1102,7 +1118,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8" t="s">
@@ -1112,8 +1128,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -1122,8 +1138,9 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
@@ -1138,8 +1155,11 @@
       <c r="F20" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
@@ -1148,8 +1168,9 @@
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="11" t="s">
@@ -1164,8 +1185,11 @@
       <c r="F22" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="G22" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
@@ -1184,8 +1208,11 @@
       <c r="F23" s="16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>66</v>
@@ -1198,8 +1225,9 @@
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>22</v>
@@ -1212,8 +1240,9 @@
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>25</v>
@@ -1226,8 +1255,9 @@
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>28</v>
@@ -1240,8 +1270,9 @@
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>31</v>
@@ -1254,8 +1285,9 @@
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>34</v>
@@ -1268,8 +1300,9 @@
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
         <v>39</v>
@@ -1286,8 +1319,11 @@
       <c r="F30" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
         <v>40</v>
@@ -1304,8 +1340,11 @@
       <c r="F31" s="17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="17" t="s">
         <v>41</v>
@@ -1322,8 +1361,11 @@
       <c r="F32" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="17" t="s">
         <v>42</v>
@@ -1340,8 +1382,11 @@
       <c r="F33" s="17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="17" t="s">
         <v>49</v>
@@ -1355,6 +1400,9 @@
       </c>
       <c r="F34" s="17" t="s">
         <v>59</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1369,7 +1417,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1382,7 +1430,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
AFDP-3021: Remove rules for adding assignee per queue
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="8196" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>RuleSet</t>
   </si>
@@ -266,21 +266,6 @@
   </si>
   <si>
     <t>setResponseDueDate, java.time.LocalDate.now().plusDays(10)</t>
-  </si>
-  <si>
-    <t>assignee, sally-acm</t>
-  </si>
-  <si>
-    <t>assignee, ian-acm</t>
-  </si>
-  <si>
-    <t>assignee, samuel-acm</t>
-  </si>
-  <si>
-    <t>assignee, ann-acm</t>
-  </si>
-  <si>
-    <t>Set Assignee</t>
   </si>
 </sst>
 </file>
@@ -951,24 +936,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125"/>
-    <col min="2" max="2" width="24.28515625"/>
-    <col min="3" max="3" width="50.140625"/>
-    <col min="4" max="4" width="100.42578125"/>
-    <col min="5" max="5" width="102.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625"/>
+    <col min="2" max="2" width="24.33203125"/>
+    <col min="3" max="3" width="50.109375"/>
+    <col min="4" max="4" width="100.44140625"/>
+    <col min="5" max="5" width="102.109375" customWidth="1"/>
     <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -978,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -988,7 +973,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -998,7 +983,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1008,7 +993,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1018,7 +1003,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1028,7 +1013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1038,7 +1023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1048,7 +1033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1058,7 +1043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1068,7 +1053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1078,7 +1063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1088,7 +1073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1098,7 +1083,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1108,7 +1093,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1118,7 +1103,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8" t="s">
@@ -1128,8 +1113,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -1138,9 +1123,8 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
@@ -1155,11 +1139,8 @@
       <c r="F20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
@@ -1168,9 +1149,8 @@
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="11" t="s">
@@ -1185,11 +1165,8 @@
       <c r="F22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
@@ -1208,11 +1185,8 @@
       <c r="F23" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>66</v>
@@ -1225,9 +1199,8 @@
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>22</v>
@@ -1240,9 +1213,8 @@
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>25</v>
@@ -1255,9 +1227,8 @@
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>28</v>
@@ -1270,9 +1241,8 @@
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>31</v>
@@ -1285,9 +1255,8 @@
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>34</v>
@@ -1300,9 +1269,8 @@
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
         <v>39</v>
@@ -1319,11 +1287,8 @@
       <c r="F30" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
         <v>40</v>
@@ -1340,11 +1305,8 @@
       <c r="F31" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G31" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="17" t="s">
         <v>41</v>
@@ -1361,11 +1323,8 @@
       <c r="F32" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G32" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="17" t="s">
         <v>42</v>
@@ -1382,11 +1341,8 @@
       <c r="F33" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="G33" s="17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="17" t="s">
         <v>49</v>
@@ -1400,9 +1356,6 @@
       </c>
       <c r="F34" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1417,7 +1370,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1430,7 +1383,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
ARKCORR-25: Fixing days in queue
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="8196" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
     <t>RuleSet</t>
   </si>
@@ -266,6 +266,42 @@
   </si>
   <si>
     <t>setResponseDueDate, java.time.LocalDate.now().plusDays(10)</t>
+  </si>
+  <si>
+    <t>Set Queue Enter Date Intake Queue</t>
+  </si>
+  <si>
+    <t>Set Queue Enter Date Fulfill Queue</t>
+  </si>
+  <si>
+    <t>Set Queue Enter Date Supervisor Approval Queue</t>
+  </si>
+  <si>
+    <t>Set Queue Enter Date Executive Approval Queue</t>
+  </si>
+  <si>
+    <t>queue?.name == "Intake" &amp;&amp; (previousQueue == null || previousQueue?.name != "Intake")</t>
+  </si>
+  <si>
+    <t>queue?.name == "Fulfill" &amp;&amp; (previousQueue == null || previousQueue?.name != "Fulfill")</t>
+  </si>
+  <si>
+    <t>queue?.name == "Supervisor Approval" &amp;&amp; (previousQueue == null || previousQueue?.name != "Supervisor Approval")</t>
+  </si>
+  <si>
+    <t>queue?.name == "Executive Approval" &amp;&amp; (previousQueue == null || previousQueue?.name != "Executive Approval")</t>
+  </si>
+  <si>
+    <t>queue?.name == "Release" &amp;&amp; (previousQueue == null || previousQueue?.name != "Release")</t>
+  </si>
+  <si>
+    <t>Set Previous Queue</t>
+  </si>
+  <si>
+    <t>queue == null || queue != null</t>
+  </si>
+  <si>
+    <t>setPreviousQueue, $caseFile.getQueue()</t>
   </si>
 </sst>
 </file>
@@ -936,24 +972,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625"/>
-    <col min="2" max="2" width="24.33203125"/>
-    <col min="3" max="3" width="50.109375"/>
-    <col min="4" max="4" width="100.44140625"/>
-    <col min="5" max="5" width="102.109375" customWidth="1"/>
-    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125"/>
+    <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="109.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.42578125"/>
+    <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -963,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -973,7 +1008,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -983,7 +1018,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -993,7 +1028,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1003,7 +1038,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1013,7 +1048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1023,7 +1058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1033,7 +1068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1043,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1053,7 +1088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1063,7 +1098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1073,7 +1108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1083,7 +1118,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1093,7 +1128,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
@@ -1103,7 +1138,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8" t="s">
@@ -1113,8 +1148,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -1122,9 +1157,8 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
@@ -1136,21 +1170,17 @@
       <c r="E20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="4"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="11" t="s">
@@ -1160,13 +1190,10 @@
         <v>17</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
@@ -1180,13 +1207,10 @@
         <v>21</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>66</v>
@@ -1198,9 +1222,8 @@
         <v>68</v>
       </c>
       <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>22</v>
@@ -1212,9 +1235,8 @@
         <v>24</v>
       </c>
       <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>25</v>
@@ -1226,9 +1248,8 @@
         <v>27</v>
       </c>
       <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>28</v>
@@ -1240,9 +1261,8 @@
         <v>30</v>
       </c>
       <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>31</v>
@@ -1254,9 +1274,8 @@
         <v>33</v>
       </c>
       <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>34</v>
@@ -1268,9 +1287,8 @@
         <v>38</v>
       </c>
       <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
         <v>39</v>
@@ -1282,13 +1300,10 @@
         <v>46</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
         <v>40</v>
@@ -1300,13 +1315,10 @@
         <v>47</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="17" t="s">
         <v>41</v>
@@ -1318,13 +1330,10 @@
         <v>48</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="17" t="s">
         <v>42</v>
@@ -1336,13 +1345,10 @@
         <v>48</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="17" t="s">
         <v>49</v>
@@ -1352,11 +1358,86 @@
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="17" t="s">
-        <v>59</v>
-      </c>
+      <c r="E35" s="17"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="17"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="17"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="17"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1370,7 +1451,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1383,7 +1464,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
ARKCORR-18: Removing assingee when object moves through queues
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t>RuleSet</t>
   </si>
@@ -194,22 +194,76 @@
     <t>Set Owning Group</t>
   </si>
   <si>
-    <t>owning group, ExecSec Intake</t>
-  </si>
-  <si>
-    <t>owning group, ExecSec Approval</t>
-  </si>
-  <si>
-    <t>owning group, ExecSec Release</t>
+    <t>com.armedia.acm.services.participants.model.AcmAssignedObject</t>
+  </si>
+  <si>
+    <t>com.armedia.acm.services.participants.model.AcmParticipant</t>
+  </si>
+  <si>
+    <t>Set Response Due Date</t>
+  </si>
+  <si>
+    <t>responseDueDate == null</t>
+  </si>
+  <si>
+    <t>setResponseDueDate, java.time.LocalDate.now().plusDays(10)</t>
+  </si>
+  <si>
+    <t>Set Queue Enter Date Intake Queue</t>
+  </si>
+  <si>
+    <t>Set Queue Enter Date Fulfill Queue</t>
+  </si>
+  <si>
+    <t>Set Queue Enter Date Supervisor Approval Queue</t>
+  </si>
+  <si>
+    <t>Set Queue Enter Date Executive Approval Queue</t>
+  </si>
+  <si>
+    <t>queue?.name == "Intake" &amp;&amp; (previousQueue == null || previousQueue?.name != "Intake")</t>
+  </si>
+  <si>
+    <t>queue?.name == "Fulfill" &amp;&amp; (previousQueue == null || previousQueue?.name != "Fulfill")</t>
+  </si>
+  <si>
+    <t>queue?.name == "Supervisor Approval" &amp;&amp; (previousQueue == null || previousQueue?.name != "Supervisor Approval")</t>
+  </si>
+  <si>
+    <t>queue?.name == "Executive Approval" &amp;&amp; (previousQueue == null || previousQueue?.name != "Executive Approval")</t>
+  </si>
+  <si>
+    <t>queue?.name == "Release" &amp;&amp; (previousQueue == null || previousQueue?.name != "Release")</t>
+  </si>
+  <si>
+    <t>Set Previous Queue</t>
+  </si>
+  <si>
+    <t>queue == null || queue != null</t>
+  </si>
+  <si>
+    <t>setPreviousQueue, $caseFile.getQueue()</t>
   </si>
   <si>
     <t>addOrUpdateParticipant($caseFile, "$1", "$2");</t>
   </si>
   <si>
-    <t>com.armedia.acm.services.participants.model.AcmAssignedObject</t>
-  </si>
-  <si>
-    <t>com.armedia.acm.services.participants.model.AcmParticipant</t>
+    <t>owning group, new String('ExecSec Intake')</t>
+  </si>
+  <si>
+    <t>owning group, new String('Analyst - AG')</t>
+  </si>
+  <si>
+    <t>owning group, new String('Supervisor - AG')</t>
+  </si>
+  <si>
+    <t>owning group, new String('ExecSec Approval')</t>
+  </si>
+  <si>
+    <t>owning group, new String('ExecSec Release')</t>
+  </si>
+  <si>
+    <t>assignee, new String('')</t>
   </si>
   <si>
     <t>function String dateFormat(String fmt)
@@ -228,8 +282,12 @@
     Boolean evaluated = exp.getValue(ec, obj, Boolean.class);
     return evaluated;
 }
-function void addOrUpdateParticipant(AcmAssignedObject obj, String type, String id) 
+function void addOrUpdateParticipant(AcmAssignedObject obj, String type, String expression) 
 {
+    ExpressionParser ep = new SpelExpressionParser();
+    Expression exp = ep.parseExpression(expression);
+    EvaluationContext ec = new StandardEvaluationContext();
+    String id = exp.getValue(ec, obj, String.class);
     if  (obj.getParticipants() != null &amp;&amp; type != null)
     {
         boolean updated = false;
@@ -251,57 +309,6 @@
         }
     }
 }</t>
-  </si>
-  <si>
-    <t>owning group, Analyst - AG</t>
-  </si>
-  <si>
-    <t>owning group, Supervisor - AG</t>
-  </si>
-  <si>
-    <t>Set Response Due Date</t>
-  </si>
-  <si>
-    <t>responseDueDate == null</t>
-  </si>
-  <si>
-    <t>setResponseDueDate, java.time.LocalDate.now().plusDays(10)</t>
-  </si>
-  <si>
-    <t>Set Queue Enter Date Intake Queue</t>
-  </si>
-  <si>
-    <t>Set Queue Enter Date Fulfill Queue</t>
-  </si>
-  <si>
-    <t>Set Queue Enter Date Supervisor Approval Queue</t>
-  </si>
-  <si>
-    <t>Set Queue Enter Date Executive Approval Queue</t>
-  </si>
-  <si>
-    <t>queue?.name == "Intake" &amp;&amp; (previousQueue == null || previousQueue?.name != "Intake")</t>
-  </si>
-  <si>
-    <t>queue?.name == "Fulfill" &amp;&amp; (previousQueue == null || previousQueue?.name != "Fulfill")</t>
-  </si>
-  <si>
-    <t>queue?.name == "Supervisor Approval" &amp;&amp; (previousQueue == null || previousQueue?.name != "Supervisor Approval")</t>
-  </si>
-  <si>
-    <t>queue?.name == "Executive Approval" &amp;&amp; (previousQueue == null || previousQueue?.name != "Executive Approval")</t>
-  </si>
-  <si>
-    <t>queue?.name == "Release" &amp;&amp; (previousQueue == null || previousQueue?.name != "Release")</t>
-  </si>
-  <si>
-    <t>Set Previous Queue</t>
-  </si>
-  <si>
-    <t>queue == null || queue != null</t>
-  </si>
-  <si>
-    <t>setPreviousQueue, $caseFile.getQueue()</t>
   </si>
 </sst>
 </file>
@@ -974,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1122,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,7 +1132,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -1135,7 +1142,7 @@
         <v>10</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1190,7 +1197,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1213,13 +1220,13 @@
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E24" s="17"/>
     </row>
@@ -1300,7 +1307,7 @@
         <v>46</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1315,7 +1322,7 @@
         <v>47</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,7 +1337,7 @@
         <v>48</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1345,7 +1352,7 @@
         <v>48</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,90 +1365,100 @@
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="17" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="17"/>
+      <c r="E35" s="17" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="17" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="17"/>
+      <c r="E36" s="17" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="17"/>
+      <c r="E37" s="17" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="17" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="17"/>
+      <c r="E38" s="17" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="17" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="17"/>
+      <c r="E39" s="17" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="17" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E40" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ARKCORR-18 Use regular LDAP groups as owning group, versus ad-hoc groups.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-correspondence.xlsx
+++ b/acm/rules/drools-case-file-rules-correspondence.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmiller\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -246,21 +246,6 @@
   </si>
   <si>
     <t>addOrUpdateParticipant($caseFile, "$1", "$2");</t>
-  </si>
-  <si>
-    <t>owning group, new String('ExecSec Intake')</t>
-  </si>
-  <si>
-    <t>owning group, new String('Analyst - AG')</t>
-  </si>
-  <si>
-    <t>owning group, new String('Supervisor - AG')</t>
-  </si>
-  <si>
-    <t>owning group, new String('ExecSec Approval')</t>
-  </si>
-  <si>
-    <t>owning group, new String('ExecSec Release')</t>
   </si>
   <si>
     <t>assignee, new String('')</t>
@@ -309,6 +294,21 @@
         }
     }
 }</t>
+  </si>
+  <si>
+    <t>owning group, new String('ANALYST - AG')</t>
+  </si>
+  <si>
+    <t>owning group, new String('EXECSEC APPROVAL')</t>
+  </si>
+  <si>
+    <t>owning group, new String('EXECSEC RELEASE')</t>
+  </si>
+  <si>
+    <t>owning group, new String('EXECSEC INTAKE')</t>
+  </si>
+  <si>
+    <t>owning group, new String('SUPERVISOR - AG')</t>
   </si>
 </sst>
 </file>
@@ -981,21 +981,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125"/>
-    <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="109.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="100.42578125"/>
+    <col min="1" max="1" width="19.453125"/>
+    <col min="2" max="2" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="109.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.453125"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -1005,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -1015,7 +1015,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -1025,7 +1025,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -1035,7 +1035,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -1045,7 +1045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -1055,7 +1055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -1065,7 +1065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -1075,7 +1075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -1085,7 +1085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -1095,7 +1095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1105,7 +1105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1115,7 +1115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1125,7 +1125,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -1135,17 +1135,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8" t="s">
@@ -1155,8 +1155,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -1165,7 +1165,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
@@ -1178,7 +1178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
@@ -1187,7 +1187,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="11" t="s">
@@ -1200,7 +1200,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>59</v>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="E24" s="17"/>
     </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>22</v>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="E25" s="17"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>25</v>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="E26" s="17"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>28</v>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="E27" s="17"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>31</v>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="E28" s="17"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>34</v>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="E29" s="17"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
         <v>39</v>
@@ -1307,10 +1307,10 @@
         <v>46</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
         <v>40</v>
@@ -1322,10 +1322,10 @@
         <v>47</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="17" t="s">
         <v>41</v>
@@ -1337,10 +1337,10 @@
         <v>48</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="17" t="s">
         <v>42</v>
@@ -1355,7 +1355,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="17" t="s">
         <v>49</v>
@@ -1368,7 +1368,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="17" t="s">
         <v>62</v>
@@ -1380,10 +1380,10 @@
         <v>55</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="17" t="s">
         <v>63</v>
@@ -1395,10 +1395,10 @@
         <v>55</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="17" t="s">
         <v>64</v>
@@ -1410,10 +1410,10 @@
         <v>55</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="17" t="s">
         <v>65</v>
@@ -1425,10 +1425,10 @@
         <v>55</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="17" t="s">
         <v>62</v>
@@ -1440,10 +1440,10 @@
         <v>55</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="17" t="s">
         <v>71</v>
@@ -1468,7 +1468,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1481,7 +1481,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>